<commit_message>
updates to the README and addition of the Alenxandria Convention format for ontologies
</commit_message>
<xml_diff>
--- a/Templates/GEO-templates/MIATE_GEOSubmissionFields.xlsx
+++ b/Templates/GEO-templates/MIATE_GEOSubmissionFields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/MIATE/GEO-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/MIATE/Templates/GEO-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{0B9E77D0-BE7F-4E17-835F-E3690CF90F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21D724A9-AC61-4FAC-9102-861D350E0618}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{0B9E77D0-BE7F-4E17-835F-E3690CF90F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7331208-A404-4469-8C02-BF879375005C}"/>
   <bookViews>
-    <workbookView xWindow="60510" yWindow="2670" windowWidth="18405" windowHeight="9885" xr2:uid="{96D632C3-BC33-40DC-B65D-F5E5B768A162}"/>
+    <workbookView xWindow="29340" yWindow="960" windowWidth="25200" windowHeight="13650" xr2:uid="{96D632C3-BC33-40DC-B65D-F5E5B768A162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -955,7 +955,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>Sample name</t>
   </si>
@@ -1393,24 +1393,12 @@
     <t>Mus musculus</t>
   </si>
   <si>
-    <t>UBERON:0002107</t>
-  </si>
-  <si>
-    <t>NCBITAXON:10090</t>
-  </si>
-  <si>
     <t>C57BL/6</t>
   </si>
   <si>
-    <t>MGI:2159769</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>PATO:0000384</t>
-  </si>
-  <si>
     <t>day</t>
   </si>
   <si>
@@ -1420,15 +1408,9 @@
     <t>degree celsius</t>
   </si>
   <si>
-    <t>UO:0000027</t>
-  </si>
-  <si>
     <t>percent</t>
   </si>
   <si>
-    <t>UO:0000187</t>
-  </si>
-  <si>
     <t>Innovive cage</t>
   </si>
   <si>
@@ -1447,9 +1429,6 @@
     <t>2,3,7,8-tetrachlorodibenzodioxine</t>
   </si>
   <si>
-    <t>CHEBI:28119</t>
-  </si>
-  <si>
     <t>Accustandard</t>
   </si>
   <si>
@@ -2084,6 +2063,33 @@
       </rPr>
       <t>light_cycle</t>
     </r>
+  </si>
+  <si>
+    <t>UBERON_0002107</t>
+  </si>
+  <si>
+    <t>NCBITAXON_10090</t>
+  </si>
+  <si>
+    <t>MGI_2159769</t>
+  </si>
+  <si>
+    <t>PATO_0000384</t>
+  </si>
+  <si>
+    <t>UO_0000033</t>
+  </si>
+  <si>
+    <t>UO_0000027</t>
+  </si>
+  <si>
+    <t>UO_0000187</t>
+  </si>
+  <si>
+    <t>12_12_00 PM</t>
+  </si>
+  <si>
+    <t>CHEBI_28119</t>
   </si>
 </sst>
 </file>
@@ -2541,8 +2547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5AC006-0FEF-487B-9E31-F6371844BA9A}">
   <dimension ref="A1:BN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="BL2" sqref="BL2"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2570,7 +2576,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -2585,7 +2591,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -2594,28 +2600,28 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>11</v>
@@ -2624,16 +2630,16 @@
         <v>12</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>14</v>
@@ -2645,19 +2651,19 @@
         <v>16</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>17</v>
@@ -2666,19 +2672,19 @@
         <v>18</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>19</v>
@@ -2690,10 +2696,10 @@
         <v>21</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>22</v>
@@ -2702,13 +2708,13 @@
         <v>23</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>24</v>
@@ -2726,39 +2732,39 @@
         <v>28</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="BN1" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
@@ -2770,37 +2776,37 @@
         <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="L2" s="5" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="M2" s="5">
         <v>4</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="P2" s="6">
         <v>28</v>
@@ -2809,145 +2815,145 @@
         <v>56</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="T2" s="2">
         <v>23</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="W2" s="2">
         <v>35</v>
       </c>
       <c r="X2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>0.5083333333333333</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="AG2" s="6">
         <v>8940</v>
       </c>
       <c r="AH2" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="AO2" s="2">
         <v>321.96976000000001</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="AR2" s="6">
         <v>99.8</v>
       </c>
       <c r="AT2" s="9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="AU2" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AV2" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="AW2" s="10">
         <v>0.1</v>
       </c>
       <c r="AX2" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="AY2" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AZ2" s="9">
         <v>4</v>
       </c>
       <c r="BA2" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="BB2" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="BC2" s="9">
         <v>7</v>
       </c>
       <c r="BD2" s="10" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="BE2" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="BF2" s="10">
         <v>0</v>
       </c>
       <c r="BG2" s="10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="BH2" s="10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="BI2" s="10">
         <v>28</v>
       </c>
       <c r="BJ2" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="BK2" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="BL2" s="10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="BM2" s="10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.2">

</xml_diff>